<commit_message>
EPBDS-13196 Add more tests for where keyword
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8954_WhereKeyword.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8954_WhereKeyword.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\workspaces\.openl1\user-workspace\admin\test1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekosolapova/work/demoMaster/openl-demo/user-workspace/DEFAULT/EPBDS-8954_WhereKeyword/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38DB768-24D6-48C4-A3BE-AAD7EDCCB47D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA394914-4ED7-4A41-96FD-7C676F68D433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="4" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Tests" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_Toc407014249" localSheetId="1">Calculation!$I$4</definedName>
+    <definedName name="_Toc407014249" localSheetId="1">Calculation!$J$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="82">
   <si>
     <t>Steps</t>
   </si>
@@ -49,6 +49,166 @@
   </si>
   <si>
     <t>limitDefinedByUser</t>
+  </si>
+  <si>
+    <t>= (Agreed Value of the vehicle - Market Value of the vehicle) / Market Value of the vehicle is more than Limit Defined By User</t>
+  </si>
+  <si>
+    <t>Test whereKeyword whereKeywordTest</t>
+  </si>
+  <si>
+    <t>_res_</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>vehicle.agreedValue</t>
+  </si>
+  <si>
+    <t>vehicle.marketValue</t>
+  </si>
+  <si>
+    <t>Agreed Value</t>
+  </si>
+  <si>
+    <t>Market Value</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Limit Defined By User</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>Test identifierSequence identifierSequenceTest</t>
+  </si>
+  <si>
+    <t>Notation of Explanatory Variables</t>
+  </si>
+  <si>
+    <t>BEX supports a notation where an expression is written using simple variables followed by the attributes they represent. For example, assume that the following expression is used in Java:</t>
+  </si>
+  <si>
+    <t>(Agreed Value of the vehicle - Market Value of the vehicle) / Market Value of the vehicle is more than Limit Defined By User</t>
+  </si>
+  <si>
+    <t>The expression is hard to read. However, it becomes much simpler if written according to the notion of explanatory variables as follows:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(A - M) / M &gt; X, where </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  A - Agreed Value of the vehicle, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  M - Market Value of the vehicle, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  X - Limit Defined By User</t>
+  </si>
+  <si>
+    <t>This syntax is similar to the one used in scientific publications and is much easier to read for complex expressions. It provides a good mix of mathematical clarity and business readability.</t>
+  </si>
+  <si>
+    <t>Spreadsheet boolean identifierSequence(Vehicle vehicle, BigDecimal limitDefinedByUser)</t>
+  </si>
+  <si>
+    <t>Spreadsheet boolean whereKeyword(Vehicle vehicle, BigDecimal limitDefinedByUser)</t>
+  </si>
+  <si>
+    <t>RET1</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>Double localParameter</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>P1==P2, where P1 - Local Parameter, P2 - My Parameter</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>Rules Double myRules(Double myParameter, Date  inputDate)</t>
+  </si>
+  <si>
+    <t>DateRange dRangeYes</t>
+  </si>
+  <si>
+    <t>DateRange dRangeNo</t>
+  </si>
+  <si>
+    <t>Date Yes</t>
+  </si>
+  <si>
+    <t>Date No</t>
+  </si>
+  <si>
+    <t>1/1/2001 - 1/1/2002</t>
+  </si>
+  <si>
+    <t>1/1/2003 - 1/1/2004</t>
+  </si>
+  <si>
+    <t>1/1/2005 - 1/1/2006</t>
+  </si>
+  <si>
+    <t>01/02/2001-01/03/2001</t>
+  </si>
+  <si>
+    <t>01/02/2003-01/03/2003</t>
+  </si>
+  <si>
+    <t>01/02/2005-01/03/2005</t>
+  </si>
+  <si>
+    <t>contains( d1, d)&amp;&amp;!contains( d2, d), where d - Input date, d1 - dRangeYes, d2 -dRangeNo</t>
+  </si>
+  <si>
+    <t>Test myRules myRulesTest</t>
+  </si>
+  <si>
+    <t>myParameter</t>
+  </si>
+  <si>
+    <t>inputDate</t>
+  </si>
+  <si>
+    <t>//Complex condition</t>
+  </si>
+  <si>
+    <t>//"Where" expression is in result</t>
+  </si>
+  <si>
+    <t>Double outParam</t>
+  </si>
+  <si>
+    <t>Rules Double myRules2(Double myParameter)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double </t>
+  </si>
+  <si>
+    <t>a+b,
+ where a - myParameter, b - outParam</t>
+  </si>
+  <si>
+    <t>// "Where" keyword is user in the external conditions</t>
   </si>
   <si>
     <t>=(A - M) / M &gt; X, where
@@ -57,83 +217,71 @@
     X - Limit Defined By User</t>
   </si>
   <si>
-    <t>= (Agreed Value of the vehicle - Market Value of the vehicle) / Market Value of the vehicle is more than Limit Defined By User</t>
-  </si>
-  <si>
-    <t>Test whereKeyword whereKeywordTest</t>
-  </si>
-  <si>
-    <t>_res_</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>vehicle.agreedValue</t>
-  </si>
-  <si>
-    <t>vehicle.marketValue</t>
-  </si>
-  <si>
-    <t>Agreed Value</t>
-  </si>
-  <si>
-    <t>Market Value</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Limit Defined By User</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>Test identifierSequence identifierSequenceTest</t>
-  </si>
-  <si>
-    <t>Notation of Explanatory Variables</t>
-  </si>
-  <si>
-    <t>BEX supports a notation where an expression is written using simple variables followed by the attributes they represent. For example, assume that the following expression is used in Java:</t>
-  </si>
-  <si>
-    <t>(Agreed Value of the vehicle - Market Value of the vehicle) / Market Value of the vehicle is more than Limit Defined By User</t>
-  </si>
-  <si>
-    <t>The expression is hard to read. However, it becomes much simpler if written according to the notion of explanatory variables as follows:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(A - M) / M &gt; X, where </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  A - Agreed Value of the vehicle, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  M - Market Value of the vehicle, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">  X - Limit Defined By User</t>
-  </si>
-  <si>
-    <t>This syntax is similar to the one used in scientific publications and is much easier to read for complex expressions. It provides a good mix of mathematical clarity and business readability.</t>
-  </si>
-  <si>
-    <t>Spreadsheet boolean identifierSequence(Vehicle vehicle, BigDecimal limitDefinedByUser)</t>
-  </si>
-  <si>
-    <t>Spreadsheet boolean whereKeyword(Vehicle vehicle, BigDecimal limitDefinedByUser)</t>
+    <t>Conditions</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>Expression</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Returns</t>
+  </si>
+  <si>
+    <t>SmartRules Vehicle muRule3( Double agreedValue )</t>
+  </si>
+  <si>
+    <t>Double minimumValue</t>
+  </si>
+  <si>
+    <t>Double maximumValue</t>
+  </si>
+  <si>
+    <t>Double agreedValue</t>
+  </si>
+  <si>
+    <t>Agreed Condition</t>
+  </si>
+  <si>
+    <t>Vehicle return</t>
+  </si>
+  <si>
+    <t>Double marketValue</t>
+  </si>
+  <si>
+    <t>Vehicle(a, b), where a-agreedValue, b - marketValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(a&gt;=min)&amp;&amp;(a&lt;max), where a -  agreedValue, min - minimumValue, max - maximumValue </t>
+  </si>
+  <si>
+    <t>Test muRule3 muRule3Test</t>
+  </si>
+  <si>
+    <t>_res_.marketValue</t>
+  </si>
+  <si>
+    <t>_res_.agreedValue</t>
+  </si>
+  <si>
+    <t>Test myRules2 myRules2Test</t>
+  </si>
+  <si>
+    <t>My Parameter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,17 +310,51 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Courier"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -210,21 +392,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -235,9 +449,44 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -281,9 +530,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -321,7 +570,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -427,7 +676,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -603,55 +852,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE823CC0-D75F-4736-9FDB-3F4C8F4E4E68}">
   <dimension ref="B4:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="2:2" ht="21" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
+    <row r="4" spans="2:2" ht="21" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B5" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B6" s="11" t="s">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B9" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B9" s="11" t="s">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B10" s="11" t="s">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B12" s="5" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -661,27 +910,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:C16"/>
+  <dimension ref="B4:I67"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="63.21875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="63.1640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="37.5" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C4" s="19"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -689,7 +940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -697,59 +948,503 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="18"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
+      <c r="C14" s="18"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C15" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
+    <row r="16" spans="2:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B14" s="6" t="s">
+      <c r="C16" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="22"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="17"/>
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="3">
+        <v>100</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="3">
+        <v>200</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="3">
         <v>2</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>8</v>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="3">
+        <v>300</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B36" s="3">
+        <v>200</v>
+      </c>
+      <c r="C36" s="11">
+        <v>37742</v>
+      </c>
+      <c r="D36" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="9"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="G42" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="H42" s="15"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="B44" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G45" s="3">
+        <v>100</v>
+      </c>
+      <c r="H45" s="3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="3">
+        <v>300</v>
+      </c>
+      <c r="H46" s="3">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="3">
+        <v>100</v>
+      </c>
+      <c r="C47" s="3">
+        <v>1</v>
+      </c>
+      <c r="G47" s="3">
+        <v>500</v>
+      </c>
+      <c r="H47" s="3"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B48" s="3">
+        <v>200</v>
+      </c>
+      <c r="C48" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B49" s="3">
+        <v>300</v>
+      </c>
+      <c r="C49" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F54" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G54" s="14"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B55" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="F55" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B56" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" s="16"/>
+      <c r="F56" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B57" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D57" s="16"/>
+      <c r="F57" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B58" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B59" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D59" s="16"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B62" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="G62" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B63" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C63" s="17"/>
+      <c r="D63" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H63" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I63" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B64" s="3">
+        <v>100</v>
+      </c>
+      <c r="C64" s="3">
+        <v>10000</v>
+      </c>
+      <c r="D64" s="3">
+        <v>7500</v>
+      </c>
+      <c r="G64" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H64" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I64" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B65" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C65" s="3">
+        <v>30000</v>
+      </c>
+      <c r="D65" s="3">
+        <v>2000</v>
+      </c>
+      <c r="G65" s="3">
+        <v>2</v>
+      </c>
+      <c r="H65" s="3">
+        <v>2</v>
+      </c>
+      <c r="I65" s="3">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B66" s="3">
+        <v>30000</v>
+      </c>
+      <c r="C66" s="3">
+        <v>100000</v>
+      </c>
+      <c r="D66" s="3">
+        <v>50000</v>
+      </c>
+      <c r="G66" s="3">
+        <v>7777</v>
+      </c>
+      <c r="H66" s="3">
+        <v>7777</v>
+      </c>
+      <c r="I66" s="3">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3">
+        <v>90000</v>
+      </c>
+      <c r="G67" s="3">
+        <v>999999</v>
+      </c>
+      <c r="H67" s="3">
+        <v>999999</v>
+      </c>
+      <c r="I67" s="3">
+        <v>90000</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="16">
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B42:C42"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="G62:I62"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C59:D59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -764,166 +1459,166 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="3">
         <v>13</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C8" s="3">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="E8" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="3">
         <v>14</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="C9" s="3">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="E9" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="5" t="s">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
+      <c r="D14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="5" t="b">
+      <c r="E14" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="5">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="3">
         <v>13</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C15" s="3">
         <v>10</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D15" s="3">
         <v>0.3</v>
       </c>
-      <c r="E8" s="5" t="b">
+      <c r="E15" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="5">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="3">
         <v>14</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C16" s="3">
         <v>10</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D16" s="3">
         <v>0.3</v>
       </c>
-      <c r="E9" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="5">
-        <v>13</v>
-      </c>
-      <c r="C15" s="5">
-        <v>10</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="E15" s="5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="5">
-        <v>14</v>
-      </c>
-      <c r="C16" s="5">
-        <v>10</v>
-      </c>
-      <c r="D16" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="E16" s="5" t="b">
+      <c r="E16" s="3" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>